<commit_message>
se modifico tp5 db1 y de agrego el enunciado del tp5
</commit_message>
<xml_diff>
--- a/BD1/tps/tp5/punto1.xlsx
+++ b/BD1/tps/tp5/punto1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28120"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INGENIERIA EN INFORMATICA\TERCERO\segundo-cuatrimestre\BD1\tps\tp5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FACULTAD\INGENIERIA-EN-INFORMATICA\TERCERO\SEGUNDO-CUATRIMESTRE\BD1\tps\tp5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9303D1FA-74BE-47AB-8F11-CF078B7FDD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C34B7F-59F8-4DB3-BB75-4F970847E3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{EC7C85C5-CECF-413A-9DA8-2865DD4D8851}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EC7C85C5-CECF-413A-9DA8-2865DD4D8851}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="65">
   <si>
     <t>id_p</t>
   </si>
@@ -227,7 +227,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +255,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -343,17 +351,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A907454A-EDBA-4DE6-8582-A55E4BB83C85}">
   <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="F10" sqref="E10:G23"/>
+    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,27 +718,27 @@
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="10"/>
+      <c r="H2" s="12"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="10"/>
+      <c r="K2" s="12"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="10"/>
+      <c r="N2" s="12"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
     </row>
@@ -944,21 +952,21 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="10"/>
+      <c r="J9" s="12"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="7">
@@ -1136,11 +1144,11 @@
         <v>4</v>
       </c>
       <c r="K14" s="8"/>
-      <c r="L14" s="10" t="s">
+      <c r="L14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
       <c r="O14" s="8"/>
       <c r="P14" s="3"/>
     </row>
@@ -1485,67 +1493,67 @@
       <c r="P25" s="3"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="13"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="13"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="13"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
-      <c r="D83" s="13"/>
-      <c r="E83" s="13"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11"/>
     </row>
     <row r="98" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C98" s="13"/>
-      <c r="D98" s="13"/>
-      <c r="E98" s="13"/>
-      <c r="F98" s="13"/>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
+      <c r="E98" s="11"/>
+      <c r="F98" s="11"/>
+      <c r="G98" s="11"/>
+      <c r="H98" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="C98:H98"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="B47:F47"/>
@@ -1553,11 +1561,11 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="G2:H2"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="C98:H98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1566,10 +1574,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E5857C4-82AA-4671-9737-F4B2CD0A892C}">
-  <dimension ref="A1:H155"/>
+  <dimension ref="A1:H138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143:XFD143"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="C138" sqref="A138:XFD138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1578,18 +1586,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1662,12 +1670,12 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -1740,13 +1748,13 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
@@ -1776,19 +1784,14 @@
       <c r="A28" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C32" s="6" t="s">
@@ -1823,12 +1826,12 @@
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C40" s="6" t="s">
@@ -1856,12 +1859,12 @@
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C49" s="6" t="s">
@@ -1893,12 +1896,12 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="11" t="s">
+      <c r="B57" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C59" s="6" t="s">
@@ -1989,14 +1992,14 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C72" s="11" t="s">
+      <c r="C72" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D72" s="11"/>
-      <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
-      <c r="G72" s="11"/>
-      <c r="H72" s="11"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C74" s="6" t="s">
@@ -2014,7 +2017,7 @@
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C77" s="14">
+      <c r="C77" s="10">
         <v>5</v>
       </c>
     </row>
@@ -2024,12 +2027,12 @@
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="11" t="s">
+      <c r="B81" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="6" t="s">
@@ -2102,12 +2105,12 @@
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="11" t="s">
+      <c r="B90" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
-      <c r="E90" s="11"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="13"/>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="6" t="s">
@@ -2135,12 +2138,12 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B101" s="11" t="s">
+      <c r="B101" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C101" s="11"/>
-      <c r="D101" s="11"/>
-      <c r="E101" s="11"/>
+      <c r="C101" s="13"/>
+      <c r="D101" s="13"/>
+      <c r="E101" s="13"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B103" s="6" t="s">
@@ -2243,14 +2246,14 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B110" s="11" t="s">
+      <c r="B110" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C110" s="11"/>
-      <c r="D110" s="11"/>
-      <c r="E110" s="11"/>
-      <c r="F110" s="11"/>
-      <c r="G110" s="11"/>
+      <c r="C110" s="13"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="13"/>
+      <c r="F110" s="13"/>
+      <c r="G110" s="13"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B113" s="6" t="s">
@@ -2356,12 +2359,12 @@
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B125" s="11" t="s">
+      <c r="B125" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C125" s="11"/>
-      <c r="D125" s="11"/>
-      <c r="E125" s="11"/>
+      <c r="C125" s="13"/>
+      <c r="D125" s="13"/>
+      <c r="E125" s="13"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C127" s="6" t="s">
@@ -2374,13 +2377,13 @@
       </c>
     </row>
     <row r="131" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C131" s="11" t="s">
+      <c r="C131" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D131" s="11"/>
-      <c r="E131" s="11"/>
-      <c r="F131" s="11"/>
-      <c r="G131" s="11"/>
+      <c r="D131" s="13"/>
+      <c r="E131" s="13"/>
+      <c r="F131" s="13"/>
+      <c r="G131" s="13"/>
     </row>
     <row r="133" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C133" s="6" t="s">
@@ -2389,185 +2392,18 @@
     </row>
     <row r="134" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C134" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C135" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="136" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C136" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="137" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C137" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="138" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C138" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="142" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C142" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D142" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E142" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="143" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C143" s="7">
-        <v>1</v>
-      </c>
-      <c r="D143" s="7">
-        <v>1</v>
-      </c>
-      <c r="E143" s="7">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="144" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C144" s="7">
-        <v>1</v>
-      </c>
-      <c r="D144" s="7">
-        <v>2</v>
-      </c>
-      <c r="E144" s="7">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="145" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C145" s="7">
-        <v>3</v>
-      </c>
-      <c r="D145" s="7">
-        <v>1</v>
-      </c>
-      <c r="E145" s="7">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="146" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C146" s="7">
-        <v>3</v>
-      </c>
-      <c r="D146" s="7">
-        <v>1</v>
-      </c>
-      <c r="E146" s="7">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="147" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C147" s="7">
-        <v>3</v>
-      </c>
-      <c r="D147" s="7">
-        <v>4</v>
-      </c>
-      <c r="E147" s="7">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="148" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C148" s="7">
-        <v>4</v>
-      </c>
-      <c r="D148" s="7">
-        <v>1</v>
-      </c>
-      <c r="E148" s="7">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="149" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C149" s="7">
-        <v>4</v>
-      </c>
-      <c r="D149" s="7">
-        <v>6</v>
-      </c>
-      <c r="E149" s="7">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="150" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C150" s="7">
-        <v>4</v>
-      </c>
-      <c r="D150" s="7">
-        <v>6</v>
-      </c>
-      <c r="E150" s="7">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="151" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C151" s="7">
-        <v>5</v>
-      </c>
-      <c r="D151" s="7">
-        <v>1</v>
-      </c>
-      <c r="E151" s="7">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="152" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C152" s="7">
-        <v>5</v>
-      </c>
-      <c r="D152" s="7">
-        <v>1</v>
-      </c>
-      <c r="E152" s="7">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="153" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C153" s="7">
-        <v>5</v>
-      </c>
-      <c r="D153" s="7">
-        <v>4</v>
-      </c>
-      <c r="E153" s="7">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="154" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C154" s="7">
-        <v>5</v>
-      </c>
-      <c r="D154" s="7">
-        <v>5</v>
-      </c>
-      <c r="E154" s="7">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="155" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C155" s="7">
-        <v>6</v>
-      </c>
-      <c r="D155" s="7">
-        <v>6</v>
-      </c>
-      <c r="E155" s="7">
-        <v>2023</v>
-      </c>
-    </row>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138" spans="3:7" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B30:E30"/>
     <mergeCell ref="B110:G110"/>
     <mergeCell ref="B125:E125"/>
     <mergeCell ref="C131:G131"/>
@@ -2577,12 +2413,6 @@
     <mergeCell ref="B81:E81"/>
     <mergeCell ref="B90:E90"/>
     <mergeCell ref="B101:E101"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B38:E38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se completo tl tp4 de paradigmas, se agrego el tp5 y falta terminar de paradigmas. Se avanzo en el tp5 de bd1 y falta terminar
</commit_message>
<xml_diff>
--- a/BD1/tps/tp5/punto1.xlsx
+++ b/BD1/tps/tp5/punto1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FACULTAD\INGENIERIA-EN-INFORMATICA\TERCERO\SEGUNDO-CUATRIMESTRE\BD1\tps\tp5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INGENIERIA EN INFORMATICA\TERCERO\segundo-cuatrimestre\BD1\tps\tp5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C34B7F-59F8-4DB3-BB75-4F970847E3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EC273B-27FB-4263-ACB2-0B85AC8FF380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EC7C85C5-CECF-413A-9DA8-2865DD4D8851}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{EC7C85C5-CECF-413A-9DA8-2865DD4D8851}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="76">
   <si>
     <t>id_p</t>
   </si>
@@ -221,13 +221,46 @@
   </si>
   <si>
     <t>π id_a (σaño = 2021 (CU)) ∩ π id_a (σ id_m = 6 (CU))</t>
+  </si>
+  <si>
+    <t>punto g)</t>
+  </si>
+  <si>
+    <t>π id_m, materia ( (σcarga_hs &gt; 8 (M)) |×| M.id_m = id_m (FO |×| FO.id_c = C.id_c (σid_c ≥ 3 (C))) )</t>
+  </si>
+  <si>
+    <t>β &lt;-( (σid_a &gt; 2 ˄ id_a ≠ 6 (A))|×| A.id_a = CU.id_a (CU) ) |×|id_m = M.id_m (M)</t>
+  </si>
+  <si>
+    <t>ɸ &lt;- ( M |×| M.id_p = P.id_p (σtitulo = “Programador” (P)) )</t>
+  </si>
+  <si>
+    <t>πalumno, materia, año, profesor (β |×| β.id_p = ɸ.id_p ɸ)</t>
+  </si>
+  <si>
+    <t>punto h)</t>
+  </si>
+  <si>
+    <t>πalumno ((A |×| A.id_a = CU.id_a CU) / πid_a (A))</t>
+  </si>
+  <si>
+    <t>Nulo</t>
+  </si>
+  <si>
+    <t>&lt;- resultado</t>
+  </si>
+  <si>
+    <t>πalumno ((A |×| A.id_a = MT.id_a MT) / πid_c (C))</t>
+  </si>
+  <si>
+    <t>&lt;---- RESULTADO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,6 +300,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -288,7 +344,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -324,11 +380,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -354,14 +454,35 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A907454A-EDBA-4DE6-8582-A55E4BB83C85}">
   <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:G23"/>
+    <sheetView topLeftCell="A5" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,27 +839,27 @@
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="12"/>
+      <c r="H2" s="17"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="12"/>
+      <c r="K2" s="17"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="12"/>
+      <c r="N2" s="17"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
     </row>
@@ -952,21 +1073,21 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="12"/>
+      <c r="J9" s="17"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="7">
@@ -1144,11 +1265,11 @@
         <v>4</v>
       </c>
       <c r="K14" s="8"/>
-      <c r="L14" s="12" t="s">
+      <c r="L14" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
       <c r="O14" s="8"/>
       <c r="P14" s="3"/>
     </row>
@@ -1493,67 +1614,67 @@
       <c r="P25" s="3"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="11"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="11"/>
-      <c r="C83" s="11"/>
-      <c r="D83" s="11"/>
-      <c r="E83" s="11"/>
+      <c r="B83" s="18"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="18"/>
     </row>
     <row r="98" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11"/>
-      <c r="F98" s="11"/>
-      <c r="G98" s="11"/>
-      <c r="H98" s="11"/>
+      <c r="C98" s="18"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="18"/>
+      <c r="G98" s="18"/>
+      <c r="H98" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="C98:H98"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="B47:F47"/>
@@ -1561,11 +1682,11 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="C98:H98"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1574,10 +1695,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E5857C4-82AA-4671-9737-F4B2CD0A892C}">
-  <dimension ref="A1:H138"/>
+  <dimension ref="A1:J227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="C138" sqref="A138:XFD138"/>
+    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="G146" sqref="G146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,18 +1707,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="19"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1670,12 +1791,12 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -1748,13 +1869,13 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
@@ -1786,12 +1907,12 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C32" s="6" t="s">
@@ -1826,12 +1947,12 @@
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C40" s="6" t="s">
@@ -1859,12 +1980,12 @@
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C49" s="6" t="s">
@@ -1896,12 +2017,12 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="13"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C59" s="6" t="s">
@@ -1992,14 +2113,14 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C72" s="13" t="s">
+      <c r="C72" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D72" s="13"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
-      <c r="G72" s="13"/>
-      <c r="H72" s="13"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="19"/>
+      <c r="H72" s="19"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C74" s="6" t="s">
@@ -2027,12 +2148,12 @@
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="13" t="s">
+      <c r="B81" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C81" s="13"/>
-      <c r="D81" s="13"/>
-      <c r="E81" s="13"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="19"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="6" t="s">
@@ -2105,12 +2226,12 @@
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="13" t="s">
+      <c r="B90" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C90" s="13"/>
-      <c r="D90" s="13"/>
-      <c r="E90" s="13"/>
+      <c r="C90" s="19"/>
+      <c r="D90" s="19"/>
+      <c r="E90" s="19"/>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="6" t="s">
@@ -2138,12 +2259,12 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B101" s="13" t="s">
+      <c r="B101" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C101" s="13"/>
-      <c r="D101" s="13"/>
-      <c r="E101" s="13"/>
+      <c r="C101" s="19"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="19"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B103" s="6" t="s">
@@ -2246,14 +2367,14 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B110" s="13" t="s">
+      <c r="B110" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C110" s="13"/>
-      <c r="D110" s="13"/>
-      <c r="E110" s="13"/>
-      <c r="F110" s="13"/>
-      <c r="G110" s="13"/>
+      <c r="C110" s="19"/>
+      <c r="D110" s="19"/>
+      <c r="E110" s="19"/>
+      <c r="F110" s="19"/>
+      <c r="G110" s="19"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B113" s="6" t="s">
@@ -2359,12 +2480,12 @@
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B125" s="13" t="s">
+      <c r="B125" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C125" s="13"/>
-      <c r="D125" s="13"/>
-      <c r="E125" s="13"/>
+      <c r="C125" s="19"/>
+      <c r="D125" s="19"/>
+      <c r="E125" s="19"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C127" s="6" t="s">
@@ -2376,44 +2497,986 @@
         <v>13</v>
       </c>
     </row>
-    <row r="131" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C131" s="13" t="s">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C131" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="D131" s="13"/>
-      <c r="E131" s="13"/>
-      <c r="F131" s="13"/>
-      <c r="G131" s="13"/>
-    </row>
-    <row r="133" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D131" s="19"/>
+      <c r="E131" s="19"/>
+      <c r="F131" s="19"/>
+      <c r="G131" s="19"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C133" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="134" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C134" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="3:7" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B140" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C140" s="19"/>
+      <c r="D140" s="19"/>
+      <c r="E140" s="19"/>
+      <c r="F140" s="19"/>
+      <c r="G140" s="19"/>
+      <c r="H140" s="19"/>
+      <c r="I140" s="19"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B142" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C142" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B143" s="7">
+        <v>2</v>
+      </c>
+      <c r="C143" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B144" s="7">
+        <v>3</v>
+      </c>
+      <c r="C144" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="145" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B145" s="7">
+        <v>1</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="146" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B146" s="7">
+        <v>6</v>
+      </c>
+      <c r="C146" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="147" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B147" s="7">
+        <v>1</v>
+      </c>
+      <c r="C147" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="150" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B150" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C150" s="19"/>
+      <c r="D150" s="19"/>
+      <c r="E150" s="19"/>
+      <c r="F150" s="19"/>
+      <c r="G150" s="19"/>
+      <c r="H150" s="19"/>
+    </row>
+    <row r="152" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C152" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D152" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E152" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F152" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G152" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H152" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I152" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C153" s="7">
+        <v>3</v>
+      </c>
+      <c r="D153" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E153" s="7">
+        <v>1</v>
+      </c>
+      <c r="F153" s="7">
+        <v>2020</v>
+      </c>
+      <c r="G153" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H153" s="9">
+        <v>6</v>
+      </c>
+      <c r="I153" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C154" s="7">
+        <v>3</v>
+      </c>
+      <c r="D154" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E154" s="7">
+        <v>1</v>
+      </c>
+      <c r="F154" s="7">
+        <v>2021</v>
+      </c>
+      <c r="G154" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H154" s="9">
+        <v>6</v>
+      </c>
+      <c r="I154" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="155" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C155" s="7">
+        <v>3</v>
+      </c>
+      <c r="D155" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E155" s="7">
+        <v>4</v>
+      </c>
+      <c r="F155" s="7">
+        <v>2022</v>
+      </c>
+      <c r="G155" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H155" s="7">
+        <v>5</v>
+      </c>
+      <c r="I155" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C156" s="7">
+        <v>4</v>
+      </c>
+      <c r="D156" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E156" s="7">
+        <v>1</v>
+      </c>
+      <c r="F156" s="7">
+        <v>2021</v>
+      </c>
+      <c r="G156" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H156" s="9">
+        <v>6</v>
+      </c>
+      <c r="I156" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C157" s="7">
+        <v>4</v>
+      </c>
+      <c r="D157" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E157" s="7">
+        <v>6</v>
+      </c>
+      <c r="F157" s="7">
+        <v>2022</v>
+      </c>
+      <c r="G157" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H157" s="7">
+        <v>10</v>
+      </c>
+      <c r="I157" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C158" s="7">
+        <v>4</v>
+      </c>
+      <c r="D158" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E158" s="7">
+        <v>6</v>
+      </c>
+      <c r="F158" s="7">
+        <v>2023</v>
+      </c>
+      <c r="G158" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H158" s="7">
+        <v>10</v>
+      </c>
+      <c r="I158" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C159" s="7">
+        <v>5</v>
+      </c>
+      <c r="D159" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E159" s="7">
+        <v>1</v>
+      </c>
+      <c r="F159" s="7">
+        <v>2019</v>
+      </c>
+      <c r="G159" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H159" s="9">
+        <v>6</v>
+      </c>
+      <c r="I159" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C160" s="7">
+        <v>5</v>
+      </c>
+      <c r="D160" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E160" s="7">
+        <v>1</v>
+      </c>
+      <c r="F160" s="7">
+        <v>2020</v>
+      </c>
+      <c r="G160" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H160" s="9">
+        <v>6</v>
+      </c>
+      <c r="I160" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C161" s="7">
+        <v>5</v>
+      </c>
+      <c r="D161" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E161" s="7">
+        <v>4</v>
+      </c>
+      <c r="F161" s="7">
+        <v>2021</v>
+      </c>
+      <c r="G161" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H161" s="7">
+        <v>5</v>
+      </c>
+      <c r="I161" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C162" s="7">
+        <v>5</v>
+      </c>
+      <c r="D162" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E162" s="7">
+        <v>5</v>
+      </c>
+      <c r="F162" s="7">
+        <v>2021</v>
+      </c>
+      <c r="G162" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H162" s="7">
+        <v>6</v>
+      </c>
+      <c r="I162" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C165" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D165" s="19"/>
+      <c r="E165" s="19"/>
+      <c r="F165" s="19"/>
+      <c r="G165" s="19"/>
+      <c r="H165" s="19"/>
+    </row>
+    <row r="167" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C167" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D167" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E167" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F167" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G167" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H167" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I167" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C168" s="7">
+        <v>2</v>
+      </c>
+      <c r="D168" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E168" s="7">
+        <v>8</v>
+      </c>
+      <c r="F168" s="7">
+        <v>3</v>
+      </c>
+      <c r="G168" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H168" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I168" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C169" s="7">
+        <v>4</v>
+      </c>
+      <c r="D169" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E169" s="7">
+        <v>5</v>
+      </c>
+      <c r="F169" s="7">
+        <v>1</v>
+      </c>
+      <c r="G169" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H169" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I169" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C170" s="7">
+        <v>6</v>
+      </c>
+      <c r="D170" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E170" s="7">
+        <v>10</v>
+      </c>
+      <c r="F170" s="7">
+        <v>3</v>
+      </c>
+      <c r="G170" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H170" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I170" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C173" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D173" s="19"/>
+      <c r="E173" s="19"/>
+      <c r="F173" s="19"/>
+      <c r="G173" s="19"/>
+      <c r="H173" s="19"/>
+      <c r="I173" s="19"/>
+    </row>
+    <row r="175" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D175" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E175" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F175" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G175" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D176" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E176" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F176" s="7">
+        <v>2022</v>
+      </c>
+      <c r="G176" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D177" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E177" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F177" s="7">
+        <v>2022</v>
+      </c>
+      <c r="G177" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D178" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E178" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F178" s="7">
+        <v>2023</v>
+      </c>
+      <c r="G178" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D179" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E179" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F179" s="7">
+        <v>2021</v>
+      </c>
+      <c r="G179" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C183" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D183" s="19"/>
+      <c r="E183" s="19"/>
+      <c r="F183" s="19"/>
+      <c r="G183" s="19"/>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C185" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D185" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E185" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F185" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H185" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I185" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C186" s="7">
+        <v>1</v>
+      </c>
+      <c r="D186" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E186" s="7">
+        <v>1</v>
+      </c>
+      <c r="F186" s="7">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C187" s="7">
+        <v>1</v>
+      </c>
+      <c r="D187" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E187" s="7">
+        <v>2</v>
+      </c>
+      <c r="F187" s="7">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C188" s="7">
+        <v>3</v>
+      </c>
+      <c r="D188" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E188" s="7">
+        <v>1</v>
+      </c>
+      <c r="F188" s="7">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C189" s="7">
+        <v>3</v>
+      </c>
+      <c r="D189" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E189" s="7">
+        <v>1</v>
+      </c>
+      <c r="F189" s="7">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C190" s="7">
+        <v>3</v>
+      </c>
+      <c r="D190" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E190" s="7">
+        <v>4</v>
+      </c>
+      <c r="F190" s="7">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C191" s="7">
+        <v>4</v>
+      </c>
+      <c r="D191" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E191" s="7">
+        <v>1</v>
+      </c>
+      <c r="F191" s="7">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C192" s="7">
+        <v>4</v>
+      </c>
+      <c r="D192" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E192" s="7">
+        <v>6</v>
+      </c>
+      <c r="F192" s="7">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="193" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C193" s="7">
+        <v>4</v>
+      </c>
+      <c r="D193" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E193" s="7">
+        <v>6</v>
+      </c>
+      <c r="F193" s="7">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="194" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C194" s="7">
+        <v>5</v>
+      </c>
+      <c r="D194" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E194" s="7">
+        <v>1</v>
+      </c>
+      <c r="F194" s="7">
+        <v>2019</v>
+      </c>
+      <c r="I194" s="11"/>
+    </row>
+    <row r="195" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C195" s="7">
+        <v>5</v>
+      </c>
+      <c r="D195" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E195" s="7">
+        <v>1</v>
+      </c>
+      <c r="F195" s="7">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="196" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C196" s="7">
+        <v>5</v>
+      </c>
+      <c r="D196" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E196" s="7">
+        <v>4</v>
+      </c>
+      <c r="F196" s="7">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="197" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C197" s="7">
+        <v>5</v>
+      </c>
+      <c r="D197" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E197" s="7">
+        <v>5</v>
+      </c>
+      <c r="F197" s="7">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="198" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C198" s="7">
+        <v>6</v>
+      </c>
+      <c r="D198" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E198" s="7">
+        <v>6</v>
+      </c>
+      <c r="F198" s="7">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="200" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C200" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="201" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C201" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C202" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C203" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="204" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C204" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C205" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="206" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C206" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="209" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C209" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D209" s="19"/>
+      <c r="E209" s="19"/>
+      <c r="F209" s="19"/>
+      <c r="G209" s="19"/>
+    </row>
+    <row r="211" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C211" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D211" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E211" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C212" s="7">
+        <v>1</v>
+      </c>
+      <c r="D212" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E212" s="7">
+        <v>1</v>
+      </c>
+      <c r="G212" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H212" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I212" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="J212" s="21"/>
+    </row>
+    <row r="213" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C213" s="7">
+        <v>1</v>
+      </c>
+      <c r="D213" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E213" s="7">
+        <v>4</v>
+      </c>
+      <c r="G213" s="10">
+        <v>1</v>
+      </c>
+      <c r="H213" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="214" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C214" s="7">
+        <v>1</v>
+      </c>
+      <c r="D214" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E214" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C215" s="7">
+        <v>1</v>
+      </c>
+      <c r="D215" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E215" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="216" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C216" s="7">
+        <v>2</v>
+      </c>
+      <c r="D216" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E216" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C217" s="7">
+        <v>3</v>
+      </c>
+      <c r="D217" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E217" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C218" s="7">
+        <v>4</v>
+      </c>
+      <c r="D218" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E218" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C219" s="7">
+        <v>5</v>
+      </c>
+      <c r="D219" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E219" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="220" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C220" s="7">
+        <v>5</v>
+      </c>
+      <c r="D220" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E220" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C221" s="7">
+        <v>6</v>
+      </c>
+      <c r="D221" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E221" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C223" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C224" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C225" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="226" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C226" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="227" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C227" s="7">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="22">
+    <mergeCell ref="B140:I140"/>
+    <mergeCell ref="B150:H150"/>
+    <mergeCell ref="B110:G110"/>
+    <mergeCell ref="B125:E125"/>
+    <mergeCell ref="C131:G131"/>
+    <mergeCell ref="B101:E101"/>
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B110:G110"/>
-    <mergeCell ref="B125:E125"/>
-    <mergeCell ref="C131:G131"/>
     <mergeCell ref="B47:E47"/>
     <mergeCell ref="B57:E57"/>
     <mergeCell ref="C72:H72"/>
     <mergeCell ref="B81:E81"/>
     <mergeCell ref="B90:E90"/>
-    <mergeCell ref="B101:E101"/>
+    <mergeCell ref="C165:H165"/>
+    <mergeCell ref="C173:I173"/>
+    <mergeCell ref="C183:G183"/>
+    <mergeCell ref="C209:G209"/>
+    <mergeCell ref="I212:J212"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se finalizo el tp5 de bd1
</commit_message>
<xml_diff>
--- a/BD1/tps/tp5/punto1.xlsx
+++ b/BD1/tps/tp5/punto1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INGENIERIA EN INFORMATICA\TERCERO\segundo-cuatrimestre\BD1\tps\tp5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FACULTAD\INGENIERIA-EN-INFORMATICA\TERCERO\SEGUNDO-CUATRIMESTRE\BD1\tps\tp5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EC273B-27FB-4263-ACB2-0B85AC8FF380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDCA731-897A-47F9-A694-644C7E5B4358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{EC7C85C5-CECF-413A-9DA8-2865DD4D8851}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EC7C85C5-CECF-413A-9DA8-2865DD4D8851}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="75">
   <si>
     <t>id_p</t>
   </si>
@@ -251,9 +251,6 @@
   </si>
   <si>
     <t>πalumno ((A |×| A.id_a = MT.id_a MT) / πid_c (C))</t>
-  </si>
-  <si>
-    <t>&lt;---- RESULTADO</t>
   </si>
 </sst>
 </file>
@@ -309,13 +306,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -344,7 +341,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -378,26 +375,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -455,34 +432,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -799,7 +772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A907454A-EDBA-4DE6-8582-A55E4BB83C85}">
   <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="J3" sqref="J3:K7"/>
     </sheetView>
   </sheetViews>
@@ -839,27 +812,27 @@
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="17"/>
+      <c r="H2" s="16"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="17"/>
+      <c r="K2" s="16"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="17"/>
+      <c r="N2" s="16"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
     </row>
@@ -1073,21 +1046,21 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="17"/>
+      <c r="J9" s="16"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="7">
@@ -1265,11 +1238,11 @@
         <v>4</v>
       </c>
       <c r="K14" s="8"/>
-      <c r="L14" s="17" t="s">
+      <c r="L14" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
       <c r="O14" s="8"/>
       <c r="P14" s="3"/>
     </row>
@@ -1614,67 +1587,67 @@
       <c r="P25" s="3"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="18"/>
-      <c r="C64" s="18"/>
-      <c r="D64" s="18"/>
-      <c r="E64" s="18"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="18"/>
-      <c r="C73" s="18"/>
-      <c r="D73" s="18"/>
-      <c r="E73" s="18"/>
+      <c r="B73" s="15"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="18"/>
-      <c r="C83" s="18"/>
-      <c r="D83" s="18"/>
-      <c r="E83" s="18"/>
+      <c r="B83" s="15"/>
+      <c r="C83" s="15"/>
+      <c r="D83" s="15"/>
+      <c r="E83" s="15"/>
     </row>
     <row r="98" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C98" s="18"/>
-      <c r="D98" s="18"/>
-      <c r="E98" s="18"/>
-      <c r="F98" s="18"/>
-      <c r="G98" s="18"/>
-      <c r="H98" s="18"/>
+      <c r="C98" s="15"/>
+      <c r="D98" s="15"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="15"/>
+      <c r="G98" s="15"/>
+      <c r="H98" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="C98:H98"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="B47:F47"/>
@@ -1682,11 +1655,11 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="G2:H2"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="C98:H98"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1695,10 +1668,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E5857C4-82AA-4671-9737-F4B2CD0A892C}">
-  <dimension ref="A1:J227"/>
+  <dimension ref="A1:J249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
-      <selection activeCell="G146" sqref="G146"/>
+    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
+      <selection activeCell="G260" sqref="G260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,18 +1680,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="17"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1791,12 +1764,12 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -1869,13 +1842,13 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
@@ -1907,12 +1880,12 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C32" s="6" t="s">
@@ -1947,12 +1920,12 @@
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C40" s="6" t="s">
@@ -1979,35 +1952,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="19" t="s">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C48" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C49" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>7</v>
+      <c r="C49" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" s="7">
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C50" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D50" s="7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C51" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D51" s="7">
         <v>10</v>
       </c>
     </row>
@@ -2017,12 +1990,12 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="19" t="s">
+      <c r="B57" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C59" s="6" t="s">
@@ -2113,14 +2086,16 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C72" s="19" t="s">
+      <c r="A72" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D72" s="19"/>
-      <c r="E72" s="19"/>
-      <c r="F72" s="19"/>
-      <c r="G72" s="19"/>
-      <c r="H72" s="19"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="17"/>
+      <c r="F72" s="17"/>
+      <c r="G72" s="18"/>
+      <c r="H72" s="18"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C74" s="6" t="s">
@@ -2148,12 +2123,12 @@
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="19" t="s">
+      <c r="B81" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C81" s="19"/>
-      <c r="D81" s="19"/>
-      <c r="E81" s="19"/>
+      <c r="C81" s="17"/>
+      <c r="D81" s="17"/>
+      <c r="E81" s="17"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="6" t="s">
@@ -2226,12 +2201,12 @@
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="19" t="s">
+      <c r="B90" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="C90" s="19"/>
-      <c r="D90" s="19"/>
-      <c r="E90" s="19"/>
+      <c r="C90" s="17"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="17"/>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="6" t="s">
@@ -2253,1230 +2228,1265 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B101" s="19" t="s">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B107" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C101" s="19"/>
-      <c r="D101" s="19"/>
-      <c r="E101" s="19"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B103" s="6" t="s">
+      <c r="C107" s="17"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="17"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C103" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D103" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E103" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F103" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G103" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B104" s="7">
-        <v>1</v>
-      </c>
-      <c r="C104" s="7" t="s">
+      <c r="B109" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D109" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E109" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F109" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="10">
+        <v>1</v>
+      </c>
+      <c r="B110" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D104" s="7" t="s">
+      <c r="C110" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E104" s="7">
-        <v>3</v>
-      </c>
-      <c r="F104" s="7">
-        <v>2</v>
-      </c>
-      <c r="G104" s="7" t="s">
+      <c r="D110" s="14">
+        <v>3</v>
+      </c>
+      <c r="E110" s="14">
+        <v>2</v>
+      </c>
+      <c r="F110" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B105" s="7">
-        <v>1</v>
-      </c>
-      <c r="C105" s="7" t="s">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="10">
+        <v>1</v>
+      </c>
+      <c r="B111" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D105" s="7" t="s">
+      <c r="C111" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E105" s="7">
-        <v>3</v>
-      </c>
-      <c r="F105" s="7">
-        <v>3</v>
-      </c>
-      <c r="G105" s="7" t="s">
+      <c r="D111" s="14">
+        <v>3</v>
+      </c>
+      <c r="E111" s="14">
+        <v>3</v>
+      </c>
+      <c r="F111" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B106" s="7">
-        <v>3</v>
-      </c>
-      <c r="C106" s="7" t="s">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="10">
+        <v>3</v>
+      </c>
+      <c r="B112" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D106" s="7" t="s">
+      <c r="C112" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E106" s="7">
-        <v>2</v>
-      </c>
-      <c r="F106" s="7">
-        <v>2</v>
-      </c>
-      <c r="G106" s="7" t="s">
+      <c r="D112" s="14">
+        <v>2</v>
+      </c>
+      <c r="E112" s="14">
+        <v>2</v>
+      </c>
+      <c r="F112" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="7">
-        <v>3</v>
-      </c>
-      <c r="C107" s="7" t="s">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="10">
+        <v>3</v>
+      </c>
+      <c r="B113" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D107" s="7" t="s">
+      <c r="C113" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E107" s="7">
-        <v>2</v>
-      </c>
-      <c r="F107" s="7">
-        <v>3</v>
-      </c>
-      <c r="G107" s="7" t="s">
+      <c r="D113" s="14">
+        <v>2</v>
+      </c>
+      <c r="E113" s="14">
+        <v>3</v>
+      </c>
+      <c r="F113" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B110" s="19" t="s">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B116" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C110" s="19"/>
-      <c r="D110" s="19"/>
-      <c r="E110" s="19"/>
-      <c r="F110" s="19"/>
-      <c r="G110" s="19"/>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B113" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C113" s="6" t="s">
+      <c r="C116" s="17"/>
+      <c r="D116" s="17"/>
+      <c r="E116" s="17"/>
+      <c r="F116" s="17"/>
+      <c r="G116" s="17"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B119" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C119" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D113" s="6" t="s">
+      <c r="D119" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E113" s="6" t="s">
+      <c r="E119" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B114" s="7">
-        <v>1</v>
-      </c>
-      <c r="C114" s="7" t="s">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B120" s="7">
+        <v>1</v>
+      </c>
+      <c r="C120" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D114" s="9">
-        <v>1</v>
-      </c>
-      <c r="E114" s="9" t="s">
+      <c r="D120" s="9">
+        <v>1</v>
+      </c>
+      <c r="E120" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B115" s="7">
-        <v>1</v>
-      </c>
-      <c r="C115" s="7" t="s">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B121" s="7">
+        <v>1</v>
+      </c>
+      <c r="C121" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D115" s="9">
-        <v>5</v>
-      </c>
-      <c r="E115" s="7" t="s">
+      <c r="D121" s="9">
+        <v>5</v>
+      </c>
+      <c r="E121" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B116" s="7">
-        <v>2</v>
-      </c>
-      <c r="C116" s="7" t="s">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B122" s="7">
+        <v>2</v>
+      </c>
+      <c r="C122" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D116" s="9">
-        <v>1</v>
-      </c>
-      <c r="E116" s="9" t="s">
+      <c r="D122" s="9">
+        <v>1</v>
+      </c>
+      <c r="E122" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B117" s="7">
-        <v>2</v>
-      </c>
-      <c r="C117" s="7" t="s">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B123" s="7">
+        <v>2</v>
+      </c>
+      <c r="C123" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D117" s="9">
-        <v>5</v>
-      </c>
-      <c r="E117" s="7" t="s">
+      <c r="D123" s="9">
+        <v>5</v>
+      </c>
+      <c r="E123" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B118" s="7">
-        <v>3</v>
-      </c>
-      <c r="C118" s="7" t="s">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B124" s="7">
+        <v>3</v>
+      </c>
+      <c r="C124" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D118" s="9">
-        <v>1</v>
-      </c>
-      <c r="E118" s="9" t="s">
+      <c r="D124" s="9">
+        <v>1</v>
+      </c>
+      <c r="E124" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B119" s="7">
-        <v>3</v>
-      </c>
-      <c r="C119" s="7" t="s">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B125" s="7">
+        <v>3</v>
+      </c>
+      <c r="C125" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D119" s="9">
-        <v>5</v>
-      </c>
-      <c r="E119" s="7" t="s">
+      <c r="D125" s="9">
+        <v>5</v>
+      </c>
+      <c r="E125" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B125" s="19" t="s">
+    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B131" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C125" s="19"/>
-      <c r="D125" s="19"/>
-      <c r="E125" s="19"/>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C127" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C128" s="7" t="s">
+      <c r="C131" s="17"/>
+      <c r="D131" s="17"/>
+      <c r="E131" s="17"/>
+    </row>
+    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C133" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C134" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C131" s="19" t="s">
+    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B137" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D131" s="19"/>
-      <c r="E131" s="19"/>
-      <c r="F131" s="19"/>
-      <c r="G131" s="19"/>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C133" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C134" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="11" t="s">
+      <c r="C137" s="17"/>
+      <c r="D137" s="17"/>
+      <c r="E137" s="17"/>
+      <c r="F137" s="18"/>
+      <c r="G137" s="18"/>
+    </row>
+    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C139" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C140" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B140" s="19" t="s">
+    <row r="153" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C140" s="19"/>
-      <c r="D140" s="19"/>
-      <c r="E140" s="19"/>
-      <c r="F140" s="19"/>
-      <c r="G140" s="19"/>
-      <c r="H140" s="19"/>
-      <c r="I140" s="19"/>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B142" s="6" t="s">
+      <c r="B153" s="19"/>
+      <c r="C153" s="19"/>
+      <c r="D153" s="19"/>
+      <c r="E153" s="19"/>
+      <c r="F153" s="19"/>
+      <c r="G153" s="19"/>
+      <c r="H153" s="18"/>
+      <c r="I153" s="18"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A154" s="19"/>
+      <c r="B154" s="19"/>
+      <c r="C154" s="19"/>
+      <c r="D154" s="19"/>
+      <c r="E154" s="19"/>
+      <c r="F154" s="19"/>
+      <c r="G154" s="19"/>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B155" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C142" s="6" t="s">
+      <c r="C155" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B143" s="7">
-        <v>2</v>
-      </c>
-      <c r="C143" s="7" t="s">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B156" s="7">
+        <v>2</v>
+      </c>
+      <c r="C156" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B144" s="7">
-        <v>3</v>
-      </c>
-      <c r="C144" s="7" t="s">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B157" s="7">
+        <v>3</v>
+      </c>
+      <c r="C157" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="145" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B145" s="7">
-        <v>1</v>
-      </c>
-      <c r="C145" s="7" t="s">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B158" s="7">
+        <v>1</v>
+      </c>
+      <c r="C158" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="146" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B146" s="7">
-        <v>6</v>
-      </c>
-      <c r="C146" s="7" t="s">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B159" s="7">
+        <v>6</v>
+      </c>
+      <c r="C159" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="147" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B147" s="7">
-        <v>1</v>
-      </c>
-      <c r="C147" s="7" t="s">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B160" s="7">
+        <v>1</v>
+      </c>
+      <c r="C160" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="150" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B150" s="19" t="s">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A163" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C150" s="19"/>
-      <c r="D150" s="19"/>
-      <c r="E150" s="19"/>
-      <c r="F150" s="19"/>
-      <c r="G150" s="19"/>
-      <c r="H150" s="19"/>
-    </row>
-    <row r="152" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C152" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D152" s="6" t="s">
+      <c r="B163" s="17"/>
+      <c r="C163" s="17"/>
+      <c r="D163" s="17"/>
+      <c r="E163" s="17"/>
+      <c r="F163" s="17"/>
+      <c r="G163" s="17"/>
+      <c r="H163" s="18"/>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A165" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B165" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E152" s="6" t="s">
+      <c r="C165" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F152" s="6" t="s">
+      <c r="D165" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G152" s="6" t="s">
+      <c r="E165" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H152" s="6" t="s">
+      <c r="F165" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I152" s="6" t="s">
+      <c r="G165" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C153" s="7">
-        <v>3</v>
-      </c>
-      <c r="D153" s="7" t="s">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A166" s="10">
+        <v>3</v>
+      </c>
+      <c r="B166" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E153" s="7">
-        <v>1</v>
-      </c>
-      <c r="F153" s="7">
+      <c r="C166" s="14">
+        <v>1</v>
+      </c>
+      <c r="D166" s="14">
         <v>2020</v>
       </c>
-      <c r="G153" s="9" t="s">
+      <c r="E166" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="H153" s="9">
-        <v>6</v>
-      </c>
-      <c r="I153" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="154" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C154" s="7">
-        <v>3</v>
-      </c>
-      <c r="D154" s="7" t="s">
+      <c r="F166" s="20">
+        <v>6</v>
+      </c>
+      <c r="G166" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A167" s="10">
+        <v>3</v>
+      </c>
+      <c r="B167" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E154" s="7">
-        <v>1</v>
-      </c>
-      <c r="F154" s="7">
+      <c r="C167" s="14">
+        <v>1</v>
+      </c>
+      <c r="D167" s="14">
         <v>2021</v>
       </c>
-      <c r="G154" s="9" t="s">
+      <c r="E167" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="H154" s="9">
-        <v>6</v>
-      </c>
-      <c r="I154" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="155" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C155" s="7">
-        <v>3</v>
-      </c>
-      <c r="D155" s="7" t="s">
+      <c r="F167" s="20">
+        <v>6</v>
+      </c>
+      <c r="G167" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A168" s="10">
+        <v>3</v>
+      </c>
+      <c r="B168" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E155" s="7">
-        <v>4</v>
-      </c>
-      <c r="F155" s="7">
+      <c r="C168" s="14">
+        <v>4</v>
+      </c>
+      <c r="D168" s="14">
         <v>2022</v>
       </c>
-      <c r="G155" s="7" t="s">
+      <c r="E168" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H155" s="7">
-        <v>5</v>
-      </c>
-      <c r="I155" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C156" s="7">
-        <v>4</v>
-      </c>
-      <c r="D156" s="7" t="s">
+      <c r="F168" s="14">
+        <v>5</v>
+      </c>
+      <c r="G168" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A169" s="10">
+        <v>4</v>
+      </c>
+      <c r="B169" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E156" s="7">
-        <v>1</v>
-      </c>
-      <c r="F156" s="7">
+      <c r="C169" s="14">
+        <v>1</v>
+      </c>
+      <c r="D169" s="14">
         <v>2021</v>
       </c>
-      <c r="G156" s="9" t="s">
+      <c r="E169" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="H156" s="9">
-        <v>6</v>
-      </c>
-      <c r="I156" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="157" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C157" s="7">
-        <v>4</v>
-      </c>
-      <c r="D157" s="7" t="s">
+      <c r="F169" s="20">
+        <v>6</v>
+      </c>
+      <c r="G169" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A170" s="10">
+        <v>4</v>
+      </c>
+      <c r="B170" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E157" s="7">
-        <v>6</v>
-      </c>
-      <c r="F157" s="7">
+      <c r="C170" s="14">
+        <v>6</v>
+      </c>
+      <c r="D170" s="14">
         <v>2022</v>
       </c>
-      <c r="G157" s="7" t="s">
+      <c r="E170" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="H157" s="7">
+      <c r="F170" s="14">
         <v>10</v>
       </c>
-      <c r="I157" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="158" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C158" s="7">
-        <v>4</v>
-      </c>
-      <c r="D158" s="7" t="s">
+      <c r="G170" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A171" s="10">
+        <v>4</v>
+      </c>
+      <c r="B171" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E158" s="7">
-        <v>6</v>
-      </c>
-      <c r="F158" s="7">
+      <c r="C171" s="14">
+        <v>6</v>
+      </c>
+      <c r="D171" s="14">
         <v>2023</v>
       </c>
-      <c r="G158" s="7" t="s">
+      <c r="E171" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="H158" s="7">
+      <c r="F171" s="14">
         <v>10</v>
       </c>
-      <c r="I158" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="159" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C159" s="7">
-        <v>5</v>
-      </c>
-      <c r="D159" s="7" t="s">
+      <c r="G171" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A172" s="10">
+        <v>5</v>
+      </c>
+      <c r="B172" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E159" s="7">
-        <v>1</v>
-      </c>
-      <c r="F159" s="7">
+      <c r="C172" s="14">
+        <v>1</v>
+      </c>
+      <c r="D172" s="14">
         <v>2019</v>
       </c>
-      <c r="G159" s="9" t="s">
+      <c r="E172" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="H159" s="9">
-        <v>6</v>
-      </c>
-      <c r="I159" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="160" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C160" s="7">
-        <v>5</v>
-      </c>
-      <c r="D160" s="7" t="s">
+      <c r="F172" s="20">
+        <v>6</v>
+      </c>
+      <c r="G172" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A173" s="10">
+        <v>5</v>
+      </c>
+      <c r="B173" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E160" s="7">
-        <v>1</v>
-      </c>
-      <c r="F160" s="7">
+      <c r="C173" s="14">
+        <v>1</v>
+      </c>
+      <c r="D173" s="14">
         <v>2020</v>
       </c>
-      <c r="G160" s="9" t="s">
+      <c r="E173" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="H160" s="9">
-        <v>6</v>
-      </c>
-      <c r="I160" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="161" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C161" s="7">
-        <v>5</v>
-      </c>
-      <c r="D161" s="7" t="s">
+      <c r="F173" s="20">
+        <v>6</v>
+      </c>
+      <c r="G173" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A174" s="10">
+        <v>5</v>
+      </c>
+      <c r="B174" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E161" s="7">
-        <v>4</v>
-      </c>
-      <c r="F161" s="7">
+      <c r="C174" s="14">
+        <v>4</v>
+      </c>
+      <c r="D174" s="14">
         <v>2021</v>
       </c>
-      <c r="G161" s="7" t="s">
+      <c r="E174" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H161" s="7">
-        <v>5</v>
-      </c>
-      <c r="I161" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="162" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C162" s="7">
-        <v>5</v>
-      </c>
-      <c r="D162" s="7" t="s">
+      <c r="F174" s="14">
+        <v>5</v>
+      </c>
+      <c r="G174" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A175" s="10">
+        <v>5</v>
+      </c>
+      <c r="B175" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E162" s="7">
-        <v>5</v>
-      </c>
-      <c r="F162" s="7">
+      <c r="C175" s="14">
+        <v>5</v>
+      </c>
+      <c r="D175" s="14">
         <v>2021</v>
       </c>
-      <c r="G162" s="7" t="s">
+      <c r="E175" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H162" s="7">
-        <v>6</v>
-      </c>
-      <c r="I162" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="165" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C165" s="19" t="s">
+      <c r="F175" s="14">
+        <v>6</v>
+      </c>
+      <c r="G175" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A178" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D165" s="19"/>
-      <c r="E165" s="19"/>
-      <c r="F165" s="19"/>
-      <c r="G165" s="19"/>
-      <c r="H165" s="19"/>
-    </row>
-    <row r="167" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C167" s="6" t="s">
+      <c r="B178" s="17"/>
+      <c r="C178" s="17"/>
+      <c r="D178" s="17"/>
+      <c r="E178" s="17"/>
+      <c r="F178" s="17"/>
+      <c r="G178" s="17"/>
+      <c r="H178" s="18"/>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A180" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D167" s="6" t="s">
+      <c r="B180" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E167" s="6" t="s">
+      <c r="C180" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F167" s="6" t="s">
+      <c r="D180" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="G167" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H167" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I167" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="168" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C168" s="7">
-        <v>2</v>
-      </c>
-      <c r="D168" s="7" t="s">
+      <c r="E180" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F180" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G180" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A181" s="10">
+        <v>2</v>
+      </c>
+      <c r="B181" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E168" s="7">
+      <c r="C181" s="14">
         <v>8</v>
       </c>
-      <c r="F168" s="7">
-        <v>3</v>
-      </c>
-      <c r="G168" s="7" t="s">
+      <c r="D181" s="14">
+        <v>3</v>
+      </c>
+      <c r="E181" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H168" s="7" t="s">
+      <c r="F181" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I168" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="169" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C169" s="7">
-        <v>4</v>
-      </c>
-      <c r="D169" s="7" t="s">
+      <c r="G181" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A182" s="10">
+        <v>4</v>
+      </c>
+      <c r="B182" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E169" s="7">
-        <v>5</v>
-      </c>
-      <c r="F169" s="7">
-        <v>1</v>
-      </c>
-      <c r="G169" s="7" t="s">
+      <c r="C182" s="14">
+        <v>5</v>
+      </c>
+      <c r="D182" s="14">
+        <v>1</v>
+      </c>
+      <c r="E182" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H169" s="7" t="s">
+      <c r="F182" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I169" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="170" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C170" s="7">
-        <v>6</v>
-      </c>
-      <c r="D170" s="7" t="s">
+      <c r="G182" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A183" s="10">
+        <v>6</v>
+      </c>
+      <c r="B183" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E170" s="7">
+      <c r="C183" s="14">
         <v>10</v>
       </c>
-      <c r="F170" s="7">
-        <v>3</v>
-      </c>
-      <c r="G170" s="7" t="s">
+      <c r="D183" s="14">
+        <v>3</v>
+      </c>
+      <c r="E183" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H170" s="7" t="s">
+      <c r="F183" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I170" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="173" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C173" s="19" t="s">
+      <c r="G183" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A186" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="D173" s="19"/>
-      <c r="E173" s="19"/>
-      <c r="F173" s="19"/>
-      <c r="G173" s="19"/>
-      <c r="H173" s="19"/>
-      <c r="I173" s="19"/>
-    </row>
-    <row r="175" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D175" s="6" t="s">
+      <c r="B186" s="17"/>
+      <c r="C186" s="17"/>
+      <c r="D186" s="17"/>
+      <c r="E186" s="17"/>
+      <c r="F186" s="17"/>
+      <c r="G186" s="17"/>
+      <c r="H186" s="18"/>
+      <c r="I186" s="18"/>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B188" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E175" s="6" t="s">
+      <c r="C188" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F175" s="6" t="s">
+      <c r="D188" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G175" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="176" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D176" s="7" t="s">
+      <c r="E188" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B189" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E176" s="7" t="s">
+      <c r="C189" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F176" s="7">
+      <c r="D189" s="14">
         <v>2022</v>
       </c>
-      <c r="G176" s="7" t="s">
+      <c r="E189" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D177" s="7" t="s">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B190" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E177" s="7" t="s">
+      <c r="C190" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F177" s="7">
+      <c r="D190" s="14">
         <v>2022</v>
       </c>
-      <c r="G177" s="7" t="s">
+      <c r="E190" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D178" s="7" t="s">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B191" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E178" s="7" t="s">
+      <c r="C191" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F178" s="7">
+      <c r="D191" s="14">
         <v>2023</v>
       </c>
-      <c r="G178" s="7" t="s">
+      <c r="E191" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D179" s="7" t="s">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B192" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E179" s="7" t="s">
+      <c r="C192" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F179" s="7">
+      <c r="D192" s="14">
         <v>2021</v>
       </c>
-      <c r="G179" s="7" t="s">
+      <c r="E192" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C183" s="19" t="s">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B203" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D183" s="19"/>
-      <c r="E183" s="19"/>
-      <c r="F183" s="19"/>
-      <c r="G183" s="19"/>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C185" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D185" s="6" t="s">
+      <c r="C203" s="17"/>
+      <c r="D203" s="17"/>
+      <c r="E203" s="17"/>
+      <c r="F203" s="17"/>
+      <c r="G203" s="18"/>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B205" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C205" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E185" s="6" t="s">
+      <c r="D205" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F185" s="6" t="s">
+      <c r="E205" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H185" s="13" t="s">
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B206" s="10">
+        <v>1</v>
+      </c>
+      <c r="C206" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D206" s="14">
+        <v>1</v>
+      </c>
+      <c r="E206" s="14">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B207" s="10">
+        <v>1</v>
+      </c>
+      <c r="C207" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D207" s="14">
+        <v>2</v>
+      </c>
+      <c r="E207" s="14">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B208" s="10">
+        <v>3</v>
+      </c>
+      <c r="C208" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D208" s="14">
+        <v>1</v>
+      </c>
+      <c r="E208" s="14">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="209" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B209" s="10">
+        <v>3</v>
+      </c>
+      <c r="C209" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D209" s="14">
+        <v>1</v>
+      </c>
+      <c r="E209" s="14">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="210" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B210" s="10">
+        <v>3</v>
+      </c>
+      <c r="C210" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D210" s="14">
+        <v>4</v>
+      </c>
+      <c r="E210" s="14">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="211" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B211" s="10">
+        <v>4</v>
+      </c>
+      <c r="C211" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D211" s="14">
+        <v>1</v>
+      </c>
+      <c r="E211" s="14">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="212" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B212" s="10">
+        <v>4</v>
+      </c>
+      <c r="C212" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D212" s="14">
+        <v>6</v>
+      </c>
+      <c r="E212" s="14">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="213" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B213" s="10">
+        <v>4</v>
+      </c>
+      <c r="C213" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D213" s="14">
+        <v>6</v>
+      </c>
+      <c r="E213" s="14">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="214" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B214" s="10">
+        <v>5</v>
+      </c>
+      <c r="C214" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D214" s="14">
+        <v>1</v>
+      </c>
+      <c r="E214" s="14">
+        <v>2019</v>
+      </c>
+      <c r="I214" s="11"/>
+    </row>
+    <row r="215" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B215" s="10">
+        <v>5</v>
+      </c>
+      <c r="C215" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D215" s="14">
+        <v>1</v>
+      </c>
+      <c r="E215" s="14">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="216" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B216" s="10">
+        <v>5</v>
+      </c>
+      <c r="C216" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D216" s="14">
+        <v>4</v>
+      </c>
+      <c r="E216" s="14">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="217" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B217" s="10">
+        <v>5</v>
+      </c>
+      <c r="C217" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D217" s="14">
+        <v>5</v>
+      </c>
+      <c r="E217" s="14">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="218" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B218" s="10">
+        <v>6</v>
+      </c>
+      <c r="C218" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D218" s="14">
+        <v>6</v>
+      </c>
+      <c r="E218" s="14">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="220" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C220" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="221" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C221" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C222" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="223" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C223" s="7">
+        <v>3</v>
+      </c>
+      <c r="E223" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I185" s="12" t="s">
+      <c r="F223" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C186" s="7">
-        <v>1</v>
-      </c>
-      <c r="D186" s="7" t="s">
+    <row r="224" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C224" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="225" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C225" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="226" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C226" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="229" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C229" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D229" s="17"/>
+      <c r="E229" s="17"/>
+      <c r="F229" s="17"/>
+      <c r="G229" s="17"/>
+    </row>
+    <row r="231" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B231" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C231" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D231" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="232" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B232" s="10">
+        <v>1</v>
+      </c>
+      <c r="C232" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E186" s="7">
-        <v>1</v>
-      </c>
-      <c r="F186" s="7">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C187" s="7">
-        <v>1</v>
-      </c>
-      <c r="D187" s="7" t="s">
+      <c r="D232" s="14">
+        <v>1</v>
+      </c>
+      <c r="I232" s="15"/>
+      <c r="J232" s="15"/>
+    </row>
+    <row r="233" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B233" s="10">
+        <v>1</v>
+      </c>
+      <c r="C233" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E187" s="7">
-        <v>2</v>
-      </c>
-      <c r="F187" s="7">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C188" s="7">
-        <v>3</v>
-      </c>
-      <c r="D188" s="7" t="s">
+      <c r="D233" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="234" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B234" s="10">
+        <v>1</v>
+      </c>
+      <c r="C234" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D234" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="235" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B235" s="10">
+        <v>1</v>
+      </c>
+      <c r="C235" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D235" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="236" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B236" s="10">
+        <v>2</v>
+      </c>
+      <c r="C236" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D236" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="237" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B237" s="10">
+        <v>3</v>
+      </c>
+      <c r="C237" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E188" s="7">
-        <v>1</v>
-      </c>
-      <c r="F188" s="7">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C189" s="7">
-        <v>3</v>
-      </c>
-      <c r="D189" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E189" s="7">
-        <v>1</v>
-      </c>
-      <c r="F189" s="7">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C190" s="7">
-        <v>3</v>
-      </c>
-      <c r="D190" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E190" s="7">
-        <v>4</v>
-      </c>
-      <c r="F190" s="7">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C191" s="7">
-        <v>4</v>
-      </c>
-      <c r="D191" s="7" t="s">
+      <c r="D237" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B238" s="10">
+        <v>4</v>
+      </c>
+      <c r="C238" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E191" s="7">
-        <v>1</v>
-      </c>
-      <c r="F191" s="7">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C192" s="7">
-        <v>4</v>
-      </c>
-      <c r="D192" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E192" s="7">
-        <v>6</v>
-      </c>
-      <c r="F192" s="7">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="193" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C193" s="7">
-        <v>4</v>
-      </c>
-      <c r="D193" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E193" s="7">
-        <v>6</v>
-      </c>
-      <c r="F193" s="7">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="194" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C194" s="7">
-        <v>5</v>
-      </c>
-      <c r="D194" s="7" t="s">
+      <c r="D238" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="239" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B239" s="10">
+        <v>5</v>
+      </c>
+      <c r="C239" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E194" s="7">
-        <v>1</v>
-      </c>
-      <c r="F194" s="7">
-        <v>2019</v>
-      </c>
-      <c r="I194" s="11"/>
-    </row>
-    <row r="195" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C195" s="7">
-        <v>5</v>
-      </c>
-      <c r="D195" s="7" t="s">
+      <c r="D239" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B240" s="10">
+        <v>5</v>
+      </c>
+      <c r="C240" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E195" s="7">
-        <v>1</v>
-      </c>
-      <c r="F195" s="7">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="196" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C196" s="7">
-        <v>5</v>
-      </c>
-      <c r="D196" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E196" s="7">
-        <v>4</v>
-      </c>
-      <c r="F196" s="7">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="197" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C197" s="7">
-        <v>5</v>
-      </c>
-      <c r="D197" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E197" s="7">
-        <v>5</v>
-      </c>
-      <c r="F197" s="7">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="198" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C198" s="7">
-        <v>6</v>
-      </c>
-      <c r="D198" s="7" t="s">
+      <c r="D240" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B241" s="10">
+        <v>6</v>
+      </c>
+      <c r="C241" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E198" s="7">
-        <v>6</v>
-      </c>
-      <c r="F198" s="7">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="200" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C200" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="201" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C201" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="202" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C202" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="203" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C203" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="204" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C204" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="205" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C205" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="206" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C206" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="209" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C209" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="D209" s="19"/>
-      <c r="E209" s="19"/>
-      <c r="F209" s="19"/>
-      <c r="G209" s="19"/>
-    </row>
-    <row r="211" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C211" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D211" s="6" t="s">
+      <c r="D241" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="242" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B242" s="21"/>
+      <c r="C242" s="21"/>
+      <c r="D242" s="21"/>
+    </row>
+    <row r="243" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B243" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C243" s="21"/>
+      <c r="D243" s="21"/>
+    </row>
+    <row r="244" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B244" s="10">
+        <v>1</v>
+      </c>
+      <c r="C244" s="21"/>
+      <c r="D244" s="21"/>
+    </row>
+    <row r="245" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B245" s="10">
+        <v>2</v>
+      </c>
+      <c r="C245" s="21"/>
+      <c r="D245" s="21"/>
+    </row>
+    <row r="246" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B246" s="10">
+        <v>3</v>
+      </c>
+      <c r="C246" s="21"/>
+      <c r="D246" s="21"/>
+    </row>
+    <row r="247" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B247" s="10">
+        <v>4</v>
+      </c>
+      <c r="C247" s="21"/>
+      <c r="D247" s="21"/>
+    </row>
+    <row r="248" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D248" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E248" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E211" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="212" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C212" s="7">
-        <v>1</v>
-      </c>
-      <c r="D212" s="7" t="s">
+    </row>
+    <row r="249" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D249" s="10">
+        <v>1</v>
+      </c>
+      <c r="E249" s="14" t="s">
         <v>26</v>
-      </c>
-      <c r="E212" s="7">
-        <v>1</v>
-      </c>
-      <c r="G212" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H212" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="I212" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="J212" s="21"/>
-    </row>
-    <row r="213" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C213" s="7">
-        <v>1</v>
-      </c>
-      <c r="D213" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E213" s="7">
-        <v>4</v>
-      </c>
-      <c r="G213" s="10">
-        <v>1</v>
-      </c>
-      <c r="H213" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="214" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C214" s="7">
-        <v>1</v>
-      </c>
-      <c r="D214" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E214" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="215" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C215" s="7">
-        <v>1</v>
-      </c>
-      <c r="D215" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E215" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="216" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C216" s="7">
-        <v>2</v>
-      </c>
-      <c r="D216" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E216" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="217" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C217" s="7">
-        <v>3</v>
-      </c>
-      <c r="D217" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E217" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="218" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C218" s="7">
-        <v>4</v>
-      </c>
-      <c r="D218" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E218" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="219" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C219" s="7">
-        <v>5</v>
-      </c>
-      <c r="D219" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E219" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="220" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C220" s="7">
-        <v>5</v>
-      </c>
-      <c r="D220" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E220" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="221" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C221" s="7">
-        <v>6</v>
-      </c>
-      <c r="D221" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E221" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="223" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C223" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="224" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C224" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="225" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C225" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="226" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C226" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="227" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C227" s="7">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B140:I140"/>
-    <mergeCell ref="B150:H150"/>
-    <mergeCell ref="B110:G110"/>
-    <mergeCell ref="B125:E125"/>
-    <mergeCell ref="C131:G131"/>
-    <mergeCell ref="B101:E101"/>
+    <mergeCell ref="C229:G229"/>
+    <mergeCell ref="I232:J232"/>
+    <mergeCell ref="A178:G178"/>
+    <mergeCell ref="A186:G186"/>
+    <mergeCell ref="B203:F203"/>
+    <mergeCell ref="B107:E107"/>
     <mergeCell ref="B38:E38"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B46:E46"/>
     <mergeCell ref="B57:E57"/>
-    <mergeCell ref="C72:H72"/>
     <mergeCell ref="B81:E81"/>
     <mergeCell ref="B90:E90"/>
-    <mergeCell ref="C165:H165"/>
-    <mergeCell ref="C173:I173"/>
-    <mergeCell ref="C183:G183"/>
-    <mergeCell ref="C209:G209"/>
-    <mergeCell ref="I212:J212"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="B116:G116"/>
+    <mergeCell ref="B131:E131"/>
+    <mergeCell ref="B137:E137"/>
+    <mergeCell ref="A153:G154"/>
+    <mergeCell ref="A163:G163"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>